<commit_message>
- Implemented optionally including scenario metadata to Sankey visualizations (now only the name of the settings file, without path) - This can be changed using the option include_metadata (True/False, default=False)
</commit_message>
<xml_diff>
--- a/src/aiphoria/data/example_scenario.xlsx
+++ b/src/aiphoria/data/example_scenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria-pypi\src\aiphoria\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\src\aiphoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8551A4C6-99EC-459A-B811-F0743B02AC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999E48CA-8F24-43CA-BCCB-1C08627B4779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="3165" windowWidth="21600" windowHeight="11295" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="221">
   <si>
     <t>Years</t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>Path to directory where results are generated</t>
+  </si>
+  <si>
+    <t>include_metadata</t>
+  </si>
+  <si>
+    <t>Include scenario metadata (currently filename) to Sankey visualization</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,22 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1386,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}">
-  <dimension ref="A2:E36"/>
+  <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,9 +1919,34 @@
         <v>218</v>
       </c>
     </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" t="s">
+        <v>219</v>
+      </c>
+      <c r="C37" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B6:E6" xr:uid="{89FFA668-DA1A-459B-BD42-D0D7F7709F0D}"/>
   <conditionalFormatting sqref="C15:C16">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:C22">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1908,32 +1954,32 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="notEqual">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C28:C29 C24" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C21:C22 C28:C29 C24 C37" xr:uid="{79A7E31C-3284-4405-9B5F-03E099B07563}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -4841,10 +4887,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5108,6 +5154,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100806C55B750152A459818B636E97A41C3" ma:contentTypeVersion="19" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="74fd9cb75cef04cf26a1ff9ddef01b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xmlns:ns3="145cc194-9bea-4db6-b116-a042a4529fcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afbcbfdd38894bc2ff0644b00c8ec680" ns2:_="" ns3:_="">
     <xsd:import namespace="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
@@ -5370,42 +5437,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5428,9 +5463,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60021C7-CA75-4673-96EA-55284BF81134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>